<commit_message>
Changed to 104 bands (12 bands per octave)
</commit_message>
<xml_diff>
--- a/FFT-Band-Bin calculator-108B-9x12.xlsx
+++ b/FFT-Band-Bin calculator-108B-9x12.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Phil\GitHub\VisualEar 3.0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Phil\GitHub\VisualEar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{477E143F-09F5-495A-88C6-039565DE59A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C767F809-D02D-4C34-BBBC-D8077501CDD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="0" windowWidth="23040" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="7" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="60">
   <si>
     <t>Sample Rate</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>+1</t>
+  </si>
+  <si>
+    <t>12 bands per octave</t>
   </si>
 </sst>
 </file>
@@ -893,7 +896,7 @@
   <dimension ref="A2:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -935,6 +938,9 @@
       </c>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
+      <c r="F4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="13"/>
@@ -1023,8 +1029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N116"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17:G42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1334,7 +1340,7 @@
         <v>15.481865781322451</v>
       </c>
       <c r="G19" s="10">
-        <f t="shared" ref="G18:G82" si="2">F19</f>
+        <f t="shared" ref="G19:G82" si="2">F19</f>
         <v>15.481865781322451</v>
       </c>
       <c r="L19" t="s">
@@ -3966,8 +3972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633FD0B3-D6D9-4B33-AC34-91A796BF35EC}">
   <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6855,8 +6861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L116"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18:G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>